<commit_message>
updates on import exports
</commit_message>
<xml_diff>
--- a/relatedFiles/other files/services import list.xlsx
+++ b/relatedFiles/other files/services import list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Web Dev\Laravel\_Developing_Phase_Project\Murarkey Single Vendor\Murarkey_single_vendor_ecommerce_with_vuexy_template\relatedFiles\other files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94B195A4-9E0C-4339-9315-DC2400B2EFFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59072385-76CB-4474-A8FC-D824056794CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1302" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1302" uniqueCount="191">
   <si>
     <t>title</t>
   </si>
@@ -605,6 +605,9 @@
   </si>
   <si>
     <t>featured_images</t>
+  </si>
+  <si>
+    <t>HairCuts</t>
   </si>
 </sst>
 </file>
@@ -1063,8 +1066,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:L1048576"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1174,7 +1177,7 @@
         <v>132</v>
       </c>
       <c r="K2" s="11" t="s">
-        <v>17</v>
+        <v>190</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>178</v>

</xml_diff>